<commit_message>
Notas enviadas a registro
</commit_message>
<xml_diff>
--- a/OYM/_DocumentosComunes/Z_Plantilla de Evaluacion.xlsx
+++ b/OYM/_DocumentosComunes/Z_Plantilla de Evaluacion.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\DocumentosUniversitarios\OYM\_DocumentosComunes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_DESARROLLO\DocumentosUniversitarios\OYM\_DocumentosComunes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{55B04E99-3A3D-411B-ACF2-12ACA9491BBE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page 1" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Page 1'!$A$1:$O$1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Page 1'!$A$1:$G$93</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -67,16 +68,16 @@
     <t>.</t>
   </si>
   <si>
-    <t>Pract. 30</t>
+    <t>R</t>
   </si>
   <si>
-    <t>R</t>
+    <t>Pract. 40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -611,15 +612,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A1:O190"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D190" sqref="D190"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -670,10 +671,10 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
         <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>14</v>
       </c>
       <c r="M1" t="s">
         <v>10</v>
@@ -696,19 +697,19 @@
         <v>7</v>
       </c>
       <c r="D2" s="6">
-        <f>IF((N2)&gt;=70,10,"")</f>
+        <f>IF((N2)&gt;=50,10,"")</f>
         <v>10</v>
       </c>
       <c r="E2" s="2">
-        <f>IF((N2)&gt;=70,20,"")</f>
+        <f>IF((N2)&gt;=50,20,"")</f>
         <v>20</v>
       </c>
       <c r="F2" s="2">
-        <f>IF((N2)&gt;=70,20,"")</f>
+        <f>IF((N2)&gt;=50,20,"")</f>
         <v>20</v>
       </c>
       <c r="G2" s="6">
-        <f>IF((N2)&gt;=40,IF((N2-50)&gt;50,50,IF((N2-50)&lt;0,0,(N2-50))), "" )</f>
+        <f>IF((N2)&gt;=51,IF((N2-50)&gt;50,50,IF((N2-50)&lt;0,0,(N2-50))), "" )</f>
         <v>50</v>
       </c>
       <c r="H2">
@@ -722,17 +723,17 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="M2">
         <v>30</v>
       </c>
       <c r="N2">
-        <f>IF((H2+I2+J2+L2+M2+O2)&lt;70,IF((H2+I2+J2+L2+M2+O2)&gt;64,70,(H2+I2+J2+L2+M2+O2)),(H2+I2+J2+L2+M2+O2))</f>
-        <v>105</v>
+        <f>IF((H2+J2+L2+M2+O2)&lt;70,IF((H2+J2+L2+M2+O2)&gt;64,70,(H2+J2+L2+M2+O2)),(H2+J2+L2+M2+O2))</f>
+        <v>110</v>
       </c>
       <c r="O2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -740,26 +741,26 @@
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="6" t="str">
-        <f t="shared" ref="D3:D66" si="0">IF((N3)&gt;=70,10,"")</f>
+        <f t="shared" ref="D3:D66" si="0">IF((N3)&gt;=50,10,"")</f>
         <v/>
       </c>
       <c r="E3" s="2" t="str">
-        <f t="shared" ref="E3:E66" si="1">IF((N3)&gt;=70,20,"")</f>
+        <f t="shared" ref="E3:E66" si="1">IF((N3)&gt;=50,20,"")</f>
         <v/>
       </c>
       <c r="F3" s="2" t="str">
-        <f t="shared" ref="F3:F66" si="2">IF((N3)&gt;=70,20,"")</f>
+        <f t="shared" ref="F3:F66" si="2">IF((N3)&gt;=50,20,"")</f>
         <v/>
       </c>
       <c r="G3" s="6" t="str">
-        <f t="shared" ref="G3:G66" si="3">IF((N3)&gt;=40,IF((N3-50)&gt;50,50,IF((N3-50)&lt;0,0,(N3-50))), "" )</f>
+        <f t="shared" ref="G3:G66" si="3">IF((N3)&gt;=51,IF((N3-50)&gt;50,50,IF((N3-50)&lt;0,0,(N3-50))), "" )</f>
         <v/>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N66" si="4">IF((H3+I3+J3+L3+M3+O3)&lt;70,IF((H3+I3+J3+L3+M3+O3)&gt;64,70,(H3+I3+J3+L3+M3+O3)),(H3+I3+J3+L3+M3+O3))</f>
+        <f t="shared" ref="N3:N66" si="4">IF((H3+J3+L3+M3+O3)&lt;70,IF((H3+J3+L3+M3+O3)&gt;64,70,(H3+J3+L3+M3+O3)),(H3+J3+L3+M3+O3))</f>
         <v>0</v>
       </c>
     </row>
@@ -2532,26 +2533,26 @@
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
       <c r="D67" s="6" t="str">
-        <f t="shared" ref="D67:D130" si="5">IF((N67)&gt;=70,10,"")</f>
+        <f t="shared" ref="D67:D130" si="5">IF((N67)&gt;=50,10,"")</f>
         <v/>
       </c>
       <c r="E67" s="2" t="str">
-        <f t="shared" ref="E67:E130" si="6">IF((N67)&gt;=70,20,"")</f>
+        <f t="shared" ref="E67:E130" si="6">IF((N67)&gt;=50,20,"")</f>
         <v/>
       </c>
       <c r="F67" s="2" t="str">
-        <f t="shared" ref="F67:F130" si="7">IF((N67)&gt;=70,20,"")</f>
+        <f t="shared" ref="F67:F130" si="7">IF((N67)&gt;=50,20,"")</f>
         <v/>
       </c>
       <c r="G67" s="6" t="str">
-        <f t="shared" ref="G67:G130" si="8">IF((N67)&gt;=40,IF((N67-50)&gt;50,50,IF((N67-50)&lt;0,0,(N67-50))), "" )</f>
+        <f t="shared" ref="G67:G130" si="8">IF((N67)&gt;=51,IF((N67-50)&gt;50,50,IF((N67-50)&lt;0,0,(N67-50))), "" )</f>
         <v/>
       </c>
       <c r="K67">
         <v>1</v>
       </c>
       <c r="N67">
-        <f t="shared" ref="N67:N130" si="9">IF((H67+I67+J67+L67+M67+O67)&lt;70,IF((H67+I67+J67+L67+M67+O67)&gt;64,70,(H67+I67+J67+L67+M67+O67)),(H67+I67+J67+L67+M67+O67))</f>
+        <f t="shared" ref="N67:N130" si="9">IF((H67+J67+L67+M67+O67)&lt;70,IF((H67+J67+L67+M67+O67)&gt;64,70,(H67+J67+L67+M67+O67)),(H67+J67+L67+M67+O67))</f>
         <v>0</v>
       </c>
     </row>
@@ -4261,23 +4262,23 @@
     </row>
     <row r="131" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D131" s="6" t="str">
-        <f t="shared" ref="D131:D189" si="10">IF((N131)&gt;=70,10,"")</f>
+        <f t="shared" ref="D131:D179" si="10">IF((N131)&gt;=50,10,"")</f>
         <v/>
       </c>
       <c r="E131" s="2" t="str">
-        <f t="shared" ref="E131:E190" si="11">IF((N131)&gt;=70,20,"")</f>
+        <f t="shared" ref="E131:E190" si="11">IF((N131)&gt;=50,20,"")</f>
         <v/>
       </c>
       <c r="F131" s="2" t="str">
-        <f t="shared" ref="F131:F190" si="12">IF((N131)&gt;=70,20,"")</f>
+        <f t="shared" ref="F131:F190" si="12">IF((N131)&gt;=50,20,"")</f>
         <v/>
       </c>
       <c r="G131" s="6" t="str">
-        <f t="shared" ref="G131:G185" si="13">IF((N131)&gt;=40,IF((N131-50)&gt;50,50,IF((N131-50)&lt;0,0,(N131-50))), "" )</f>
+        <f t="shared" ref="G131:G190" si="13">IF((N131)&gt;=51,IF((N131-50)&gt;50,50,IF((N131-50)&lt;0,0,(N131-50))), "" )</f>
         <v/>
       </c>
       <c r="N131">
-        <f t="shared" ref="N131:N169" si="14">IF((H131+I131+J131+L131+M131+O131)&lt;70,IF((H131+I131+J131+L131+M131+O131)&gt;64,70,(H131+I131+J131+L131+M131+O131)),(H131+I131+J131+L131+M131+O131))</f>
+        <f t="shared" ref="N131:N185" si="14">IF((H131+J131+L131+M131+O131)&lt;70,IF((H131+J131+L131+M131+O131)&gt;64,70,(H131+J131+L131+M131+O131)),(H131+J131+L131+M131+O131))</f>
         <v>0</v>
       </c>
     </row>
@@ -5134,6 +5135,10 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
+      <c r="N170">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="171" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D171" s="6" t="str">
@@ -5152,6 +5157,10 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
+      <c r="N171">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="172" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D172" s="6" t="str">
@@ -5170,6 +5179,10 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
+      <c r="N172">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="173" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D173" s="6" t="str">
@@ -5188,6 +5201,10 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
+      <c r="N173">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="174" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D174" s="6" t="str">
@@ -5206,6 +5223,10 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
+      <c r="N174">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="175" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D175" s="6" t="str">
@@ -5224,6 +5245,10 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
+      <c r="N175">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="176" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D176" s="6" t="str">
@@ -5242,8 +5267,12 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
-    </row>
-    <row r="177" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="N176">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D177" s="6" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5260,8 +5289,12 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
-    </row>
-    <row r="178" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="N177">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D178" s="6" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5278,8 +5311,12 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
-    </row>
-    <row r="179" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="N178">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D179" s="6" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5296,10 +5333,14 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
-    </row>
-    <row r="180" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="N179">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D180" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="D180:D189" si="15">IF((N180)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E180" s="2" t="str">
@@ -5314,10 +5355,14 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
-    </row>
-    <row r="181" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="N180">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D181" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="E181" s="2" t="str">
@@ -5332,10 +5377,14 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
-    </row>
-    <row r="182" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="N181">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D182" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="E182" s="2" t="str">
@@ -5350,10 +5399,14 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
-    </row>
-    <row r="183" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="N182">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D183" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="E183" s="2" t="str">
@@ -5368,10 +5421,14 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
-    </row>
-    <row r="184" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="N183">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D184" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="E184" s="2" t="str">
@@ -5386,10 +5443,14 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
-    </row>
-    <row r="185" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="N184">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D185" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="E185" s="2" t="str">
@@ -5404,10 +5465,14 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
-    </row>
-    <row r="186" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="N185">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D186" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="E186" s="2" t="str">
@@ -5419,13 +5484,13 @@
         <v/>
       </c>
       <c r="G186" s="6" t="str">
-        <f t="shared" ref="G131:G190" si="15">IF((N186)&gt;=70,IF((N186-50)&gt;50,50,IF((N186-50)&lt;0,0,(N186-50))), "" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="187" spans="4:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="187" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D187" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="E187" s="2" t="str">
@@ -5437,15 +5502,15 @@
         <v/>
       </c>
       <c r="G187" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="188" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D188" s="6" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-    </row>
-    <row r="188" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D188" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
       <c r="E188" s="2" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -5455,15 +5520,15 @@
         <v/>
       </c>
       <c r="G188" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="189" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D189" s="6" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-    </row>
-    <row r="189" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D189" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
       <c r="E189" s="2" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -5473,13 +5538,13 @@
         <v/>
       </c>
       <c r="G189" s="6" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="190" spans="4:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+    </row>
+    <row r="190" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D190" s="6" t="str">
-        <f t="shared" ref="D131:D190" si="16">IF((N190)&gt;=70,10,"")</f>
+        <f t="shared" ref="D190" si="16">IF((N190)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E190" s="2" t="str">
@@ -5491,12 +5556,12 @@
         <v/>
       </c>
       <c r="G190" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1">
+  <autoFilter ref="A1:O1" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1" showButton="0"/>
     <filterColumn colId="2" showButton="0"/>
     <filterColumn colId="3" showButton="0"/>

</xml_diff>